<commit_message>
Updated route for create.handlebars file.
</commit_message>
<xml_diff>
--- a/docs/flashy_database_setup.xlsx
+++ b/docs/flashy_database_setup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\UCLA_Extension\Repo\flashy_team_prize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\UCLA_Extension\Repo\flashy_team_prize\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Users</t>
   </si>
@@ -51,12 +51,6 @@
     <t>categoryID</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -66,23 +60,35 @@
     <t>title</t>
   </si>
   <si>
-    <t>categoryName</t>
-  </si>
-  <si>
     <t>question</t>
   </si>
   <si>
     <t>answer</t>
   </si>
   <si>
-    <t>flashNumber</t>
+    <t>GREEN = belongsTo</t>
+  </si>
+  <si>
+    <t>BLUE = hasMany</t>
+  </si>
+  <si>
+    <t>displayname</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>cat_name</t>
+  </si>
+  <si>
+    <t>flash_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +117,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,11 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,80 +476,99 @@
     <col min="1" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>